<commit_message>
Added Table in Paper format
</commit_message>
<xml_diff>
--- a/Results/Results_v2.xlsx
+++ b/Results/Results_v2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helge\Documents\Deep-Learning-Lab\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCD7555-49B2-4915-9E9B-85B8E26CB68B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7805E2-5EFA-41B0-8B25-7943C3E4514E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiments" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="110">
   <si>
     <t>abs_rel</t>
   </si>
@@ -247,6 +248,114 @@
   </si>
   <si>
     <t>4ch_slic_normal_cont_normal__after_bugfix_13_2_20</t>
+  </si>
+  <si>
+    <t>Decoder</t>
+  </si>
+  <si>
+    <t>Inp. Channels</t>
+  </si>
+  <si>
+    <t>Sup. Method</t>
+  </si>
+  <si>
+    <t>Abs Rel</t>
+  </si>
+  <si>
+    <t>Sq Rel</t>
+  </si>
+  <si>
+    <t>RSME</t>
+  </si>
+  <si>
+    <t>RSME log</t>
+  </si>
+  <si>
+    <t>&lt;1.25</t>
+  </si>
+  <si>
+    <t>&lt;1.25²</t>
+  </si>
+  <si>
+    <t>&lt;1.25³</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>N2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normals </t>
+  </si>
+  <si>
+    <t>4Ch</t>
+  </si>
+  <si>
+    <t>felzenwalb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4Ch </t>
+  </si>
+  <si>
+    <t>slic</t>
+  </si>
+  <si>
+    <t>4Ch + N2D</t>
+  </si>
+  <si>
+    <t>normals</t>
+  </si>
+  <si>
+    <t>continous + normal loss</t>
+  </si>
+  <si>
+    <t>0.001 * normal</t>
+  </si>
+  <si>
+    <t>0.01 * normal</t>
+  </si>
+  <si>
+    <t>0.1 * normal</t>
+  </si>
+  <si>
+    <t>binary + normal</t>
+  </si>
+  <si>
+    <t>6Ch</t>
+  </si>
+  <si>
+    <t>4Ch + N2D + bin</t>
+  </si>
+  <si>
+    <t>3Ch + N2D + bin</t>
+  </si>
+  <si>
+    <t>4Ch + N2D + cont</t>
+  </si>
+  <si>
+    <t>3Ch + N2D + cont</t>
+  </si>
+  <si>
+    <t>4Ch + N2D +  0.001 norm</t>
+  </si>
+  <si>
+    <t>4Ch + N2D +  0.01 norm</t>
+  </si>
+  <si>
+    <t>4Ch + N2D +  0.1 norm</t>
+  </si>
+  <si>
+    <t>continous + normal</t>
+  </si>
+  <si>
+    <t>4Ch + N2D + bin + norm</t>
+  </si>
+  <si>
+    <t>3Ch+ N2D + cont + norm</t>
+  </si>
+  <si>
+    <t>4Ch + N2D + cont + norm</t>
   </si>
 </sst>
 </file>
@@ -541,73 +650,17 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <b val="0"/>
@@ -1067,74 +1120,32 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1144,13 +1155,31 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1167,23 +1196,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB54C985-E604-43C7-9B7E-5E50F7B7F72C}" name="Tabelle3" displayName="Tabelle3" ref="A2:N22" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="24" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB54C985-E604-43C7-9B7E-5E50F7B7F72C}" name="Tabelle3" displayName="Tabelle3" ref="A2:N22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="A2:N22" xr:uid="{5D97243E-7D77-486A-99EB-E71E39617BA7}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{0B897FAC-E945-495F-A663-B2C8BAD36E5C}" name="Run-Name (for the Log-file)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3ADEFB8E-AAC7-435B-9C15-1F97B755CBA2}" name="Description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{820D6FBC-2F12-45BE-B95F-1E3AF4F136B1}" name="Run-Time" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{3C47E134-A131-4E22-B3DB-C5E0FC07408D}" name="Loss Function" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{E44BF3CE-7F6A-49CF-BC07-AEE682DB45B9}" name="abs_rel" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{0BF92AC3-F9FB-4117-8433-8F5592397D9C}" name="sq_rel" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{6E63108B-CF5F-4921-8EED-826323B43A89}" name="rmse" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{5B6E3BE0-CD42-4E95-9FCA-EF74E748D81C}" name="rmse_log" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{970ED5F9-7812-4AAB-B6CE-384523A94DAB}" name="al" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{FE809ABE-BDA6-48F1-BF42-70A11636E33A}" name="a2" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{AD526890-348B-4AE3-A10C-F1EE2EF964AB}" name="a3" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{6DC31F02-CA85-4543-A877-8F519E0B81A2}" name="Scaling ratios" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{5FF9CA10-9F78-4E16-89B7-1404B14491E9}" name="med" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{73F6EE9B-92EB-4094-A8C1-BC1B906D0D51}" name="std" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0B897FAC-E945-495F-A663-B2C8BAD36E5C}" name="Run-Name (for the Log-file)" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{3ADEFB8E-AAC7-435B-9C15-1F97B755CBA2}" name="Description" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{820D6FBC-2F12-45BE-B95F-1E3AF4F136B1}" name="Run-Time" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{3C47E134-A131-4E22-B3DB-C5E0FC07408D}" name="Loss Function" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{E44BF3CE-7F6A-49CF-BC07-AEE682DB45B9}" name="abs_rel" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{0BF92AC3-F9FB-4117-8433-8F5592397D9C}" name="sq_rel" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6E63108B-CF5F-4921-8EED-826323B43A89}" name="rmse" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{5B6E3BE0-CD42-4E95-9FCA-EF74E748D81C}" name="rmse_log" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{970ED5F9-7812-4AAB-B6CE-384523A94DAB}" name="al" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{FE809ABE-BDA6-48F1-BF42-70A11636E33A}" name="a2" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{AD526890-348B-4AE3-A10C-F1EE2EF964AB}" name="a3" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{6DC31F02-CA85-4543-A877-8F519E0B81A2}" name="Scaling ratios" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{5FF9CA10-9F78-4E16-89B7-1404B14491E9}" name="med" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{73F6EE9B-92EB-4094-A8C1-BC1B906D0D51}" name="std" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1454,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,17 +1509,17 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -1535,7 +1564,7 @@
       <c r="N2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="30"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
@@ -1567,8 +1596,8 @@
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="30"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
@@ -1609,7 +1638,7 @@
       <c r="N4" s="26">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="O4" s="30"/>
+      <c r="O4" s="29"/>
     </row>
     <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
@@ -1652,7 +1681,7 @@
       <c r="N5" s="26">
         <v>0.09</v>
       </c>
-      <c r="O5" s="30"/>
+      <c r="O5" s="29"/>
     </row>
     <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
@@ -1695,7 +1724,7 @@
       <c r="N6" s="26">
         <v>9.4E-2</v>
       </c>
-      <c r="O6" s="30"/>
+      <c r="O6" s="29"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
@@ -2548,4 +2577,727 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57F043E-964E-41CF-8908-5315B29F82AD}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>0.115</v>
+      </c>
+      <c r="G2">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="H2">
+        <v>4.8630000000000004</v>
+      </c>
+      <c r="I2">
+        <v>0.193</v>
+      </c>
+      <c r="J2">
+        <v>0.877</v>
+      </c>
+      <c r="K2">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="L2">
+        <v>0.98099999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>0.123</v>
+      </c>
+      <c r="G3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="H3">
+        <v>5.0419999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.2</v>
+      </c>
+      <c r="J3">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="L3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G4">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="H4">
+        <v>5.5449999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.22</v>
+      </c>
+      <c r="J4">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="K4">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="L4">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>0.255</v>
+      </c>
+      <c r="G5">
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="H5">
+        <v>7.8920000000000003</v>
+      </c>
+      <c r="I5">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="J5">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="K5">
+        <v>9.8320000000000007</v>
+      </c>
+      <c r="L5">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>0.122</v>
+      </c>
+      <c r="G6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="H6">
+        <v>5.0259999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="L6">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G7">
+        <v>1.262</v>
+      </c>
+      <c r="H7">
+        <v>5.5510000000000002</v>
+      </c>
+      <c r="I7">
+        <v>0.22</v>
+      </c>
+      <c r="J7">
+        <v>0.83</v>
+      </c>
+      <c r="K7">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="L7">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8">
+        <v>0.443</v>
+      </c>
+      <c r="G8">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H8">
+        <v>12.083</v>
+      </c>
+      <c r="I8">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J8">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L8">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>0.443</v>
+      </c>
+      <c r="G9">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H9">
+        <v>12.083</v>
+      </c>
+      <c r="I9">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J9">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L9">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="G10">
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="H10">
+        <v>5.484</v>
+      </c>
+      <c r="I10">
+        <v>0.218</v>
+      </c>
+      <c r="J10">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="K10">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="L10">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>0.443</v>
+      </c>
+      <c r="G11">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H11">
+        <v>12.083</v>
+      </c>
+      <c r="I11">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L11">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <v>0.443</v>
+      </c>
+      <c r="G12">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H12">
+        <v>12.083</v>
+      </c>
+      <c r="I12">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J12">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L12">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G13">
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="H13">
+        <v>5.5250000000000004</v>
+      </c>
+      <c r="I13">
+        <v>0.22</v>
+      </c>
+      <c r="J13">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="K13">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="L13">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G14">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="H14">
+        <v>5.5129999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.218</v>
+      </c>
+      <c r="J14">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="K14">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="L14">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15">
+        <v>0.443</v>
+      </c>
+      <c r="G15">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H15">
+        <v>12.083</v>
+      </c>
+      <c r="I15">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J15">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K15">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L15">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16">
+        <v>0.443</v>
+      </c>
+      <c r="G16">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H16">
+        <v>12.083</v>
+      </c>
+      <c r="I16">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J16">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L16">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G17">
+        <v>1.276</v>
+      </c>
+      <c r="H17">
+        <v>5.5490000000000004</v>
+      </c>
+      <c r="I17">
+        <v>0.221</v>
+      </c>
+      <c r="J17">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="K17">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="L17">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18">
+        <v>0.443</v>
+      </c>
+      <c r="G18">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H18">
+        <v>12.083</v>
+      </c>
+      <c r="I18">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J18">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K18">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L18">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19">
+        <v>0.443</v>
+      </c>
+      <c r="G19">
+        <v>4.7569999999999997</v>
+      </c>
+      <c r="H19">
+        <v>12.083</v>
+      </c>
+      <c r="I19">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J19">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L19">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>